<commit_message>
[Front-end] feat: info page view more
when img hover, view more on info list img
</commit_message>
<xml_diff>
--- a/hyeseon_dev/cheda_data.xlsx
+++ b/hyeseon_dev/cheda_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyese\Desktop\2019_ERICA\1학년_2학기\OSS\ERICA_Cheda\hyeseon_dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slimd\OneDrive\바탕 화면\개발\오픈소스 기초 팀플\ERICA_Cheda\hyeseon_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C70B9A14-1B3B-45D0-A737-8ECB09EAE678}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C149FFFB-B410-42EF-A828-27FDE619FF13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="0" windowWidth="22620" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -803,16 +803,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -821,7 +815,13 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1987,50 +1987,50 @@
   <dimension ref="A1:IV26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="64" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A1048576"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.2" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.19921875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.69921875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="21.25" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.75" style="15" customWidth="1"/>
     <col min="3" max="3" width="31" style="15" customWidth="1"/>
-    <col min="4" max="4" width="15.09765625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="15" customWidth="1"/>
     <col min="5" max="5" width="14" style="15" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="15" customWidth="1"/>
-    <col min="7" max="7" width="40.59765625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="33.296875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="40.625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="33.25" style="13" customWidth="1"/>
     <col min="9" max="9" width="35" style="3" customWidth="1"/>
-    <col min="10" max="10" width="35.796875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.3984375" style="15" customWidth="1"/>
-    <col min="12" max="12" width="20.09765625" style="15" customWidth="1"/>
-    <col min="13" max="13" width="12.19921875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="24.19921875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="61.8984375" style="3" customWidth="1"/>
-    <col min="16" max="256" width="8.796875" style="3" customWidth="1"/>
-    <col min="257" max="16384" width="8.796875" style="4"/>
+    <col min="10" max="10" width="35.75" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.375" style="15" customWidth="1"/>
+    <col min="12" max="12" width="20.125" style="15" customWidth="1"/>
+    <col min="13" max="13" width="12.25" style="3" customWidth="1"/>
+    <col min="14" max="14" width="24.25" style="3" customWidth="1"/>
+    <col min="15" max="15" width="61.875" style="3" customWidth="1"/>
+    <col min="16" max="256" width="8.75" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="8.75" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
     </row>
-    <row r="2" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2070,13 +2070,13 @@
       <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="21"/>
+      <c r="O2" s="19"/>
     </row>
-    <row r="3" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2089,7 +2089,7 @@
       <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="16">
         <v>15000</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -2116,8 +2116,8 @@
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="17"/>
+    <row r="4" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
@@ -2128,7 +2128,7 @@
       <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="16">
         <v>20000</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -2155,8 +2155,8 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:15" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="16">
         <v>15000</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -2194,8 +2194,8 @@
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
     </row>
-    <row r="6" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2206,7 +2206,7 @@
       <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="16">
         <v>15000</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -2235,8 +2235,8 @@
       </c>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2247,7 +2247,7 @@
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="16">
         <v>15000</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -2274,8 +2274,8 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
@@ -2313,8 +2313,8 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2329,7 +2329,7 @@
       <c r="E9" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="16">
         <v>10000</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -2356,8 +2356,8 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
@@ -2370,7 +2370,7 @@
       <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="16">
         <v>100000</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -2399,8 +2399,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="18"/>
+    <row r="11" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
       <c r="B11" s="1" t="s">
         <v>60</v>
       </c>
@@ -2413,7 +2413,7 @@
       <c r="E11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="16">
         <v>150000</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -2442,8 +2442,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="16" t="s">
+    <row r="12" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2489,8 +2489,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="18"/>
+    <row r="13" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>77</v>
       </c>
@@ -2532,8 +2532,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2548,7 +2548,7 @@
       <c r="E14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="16">
         <v>60000</v>
       </c>
       <c r="G14" s="5" t="s">
@@ -2577,8 +2577,8 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
       <c r="B15" s="1" t="s">
         <v>85</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="E15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="16">
         <v>60000</v>
       </c>
       <c r="G15" s="7" t="s">
@@ -2620,8 +2620,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
       <c r="B16" s="1" t="s">
         <v>88</v>
       </c>
@@ -2663,8 +2663,8 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21"/>
       <c r="B17" s="1" t="s">
         <v>93</v>
       </c>
@@ -2706,8 +2706,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21"/>
       <c r="B18" s="1" t="s">
         <v>98</v>
       </c>
@@ -2749,8 +2749,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
       <c r="B19" s="1" t="s">
         <v>103</v>
       </c>
@@ -2794,8 +2794,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:15" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>110</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2841,8 +2841,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="17"/>
+    <row r="21" spans="1:15" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
       <c r="B21" s="1" t="s">
         <v>116</v>
       </c>
@@ -2886,8 +2886,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="17"/>
+    <row r="22" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
       <c r="B22" s="1" t="s">
         <v>119</v>
       </c>
@@ -2931,8 +2931,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
       <c r="B23" s="1" t="s">
         <v>120</v>
       </c>
@@ -2976,8 +2976,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
       <c r="B24" s="1" t="s">
         <v>122</v>
       </c>
@@ -3021,8 +3021,8 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
         <v>125</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -3066,8 +3066,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="18"/>
+    <row r="26" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
       <c r="B26" s="1" t="s">
         <v>135</v>
       </c>
@@ -3113,14 +3113,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>